<commit_message>
more raw numbers for figures
</commit_message>
<xml_diff>
--- a/events_figs/f5_supplements/asymp_predictors.xlsx
+++ b/events_figs/f5_supplements/asymp_predictors.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>pearson</t>
   </si>
@@ -31,6 +31,84 @@
   </si>
   <si>
     <t>adjr2_agg</t>
+  </si>
+  <si>
+    <t>pearson</t>
+  </si>
+  <si>
+    <t>pearson_p</t>
+  </si>
+  <si>
+    <t>adjr2</t>
+  </si>
+  <si>
+    <t>pearson_agg</t>
+  </si>
+  <si>
+    <t>pearson_p_agg</t>
+  </si>
+  <si>
+    <t>adjr2_agg</t>
+  </si>
+  <si>
+    <t>pearson</t>
+  </si>
+  <si>
+    <t>pearson_p</t>
+  </si>
+  <si>
+    <t>adjr2</t>
+  </si>
+  <si>
+    <t>pearson_agg</t>
+  </si>
+  <si>
+    <t>pearson_p_agg</t>
+  </si>
+  <si>
+    <t>adjr2_agg</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>signal_var_norm</t>
+  </si>
+  <si>
+    <t>num_neurons</t>
+  </si>
+  <si>
+    <t>corr_cos2_area</t>
+  </si>
+  <si>
+    <t>cos2_area</t>
+  </si>
+  <si>
+    <t>signal_density</t>
+  </si>
+  <si>
+    <t>noise_density</t>
+  </si>
+  <si>
+    <t>eigen_noise_ipr</t>
+  </si>
+  <si>
+    <t>signal_var</t>
+  </si>
+  <si>
+    <t>var_fwhm_cm</t>
+  </si>
+  <si>
+    <t>num_trials</t>
+  </si>
+  <si>
+    <t>loadings_ipr</t>
+  </si>
+  <si>
+    <t>avg_signal</t>
+  </si>
+  <si>
+    <t>corr_loadings_ipr</t>
   </si>
   <si>
     <t>pearson</t>
@@ -69,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -79,14 +157,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,274 +178,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="true"/>
-    <col min="2" max="2" width="15.7109375" customWidth="true"/>
-    <col min="3" max="3" width="14.7109375" customWidth="true"/>
-    <col min="4" max="4" width="13.42578125" customWidth="true"/>
-    <col min="5" max="5" width="14.7109375" customWidth="true"/>
-    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="true"/>
+    <col min="2" max="2" width="13.42578125" customWidth="true"/>
+    <col min="3" max="3" width="15.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="5" max="5" width="13.42578125" customWidth="true"/>
+    <col min="6" max="6" width="14.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
+      <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0">
         <v>0.75618507345519581</v>
       </c>
-      <c r="B2" s="0">
+      <c r="C2" s="0">
         <v>1.5917456728403616e-14</v>
       </c>
-      <c r="C2" s="0">
+      <c r="D2" s="0">
         <v>0.56569894910667484</v>
       </c>
-      <c r="D2" s="0">
+      <c r="E2" s="0">
         <v>0.83145769687469295</v>
       </c>
-      <c r="E2" s="0">
+      <c r="F2" s="0">
         <v>0.0028652427191023506</v>
       </c>
-      <c r="F2" s="0">
+      <c r="G2" s="0">
         <v>0.65273713940368983</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
+      <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0">
         <v>-0.54097961361342106</v>
       </c>
-      <c r="B3" s="0">
+      <c r="C3" s="0">
         <v>9.292275674611443e-07</v>
       </c>
-      <c r="C3" s="0">
+      <c r="D3" s="0">
         <v>0.28255407009311662</v>
       </c>
-      <c r="D3" s="0">
+      <c r="E3" s="0">
         <v>-0.61451955808722858</v>
       </c>
-      <c r="E3" s="0">
+      <c r="F3" s="0">
         <v>0.058698413577875502</v>
       </c>
-      <c r="F3" s="0">
+      <c r="G3" s="0">
         <v>0.29983857318068796</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="0">
         <v>-0.41677572122806306</v>
       </c>
-      <c r="B4" s="0">
+      <c r="C4" s="0">
         <v>0.00027077624123422847</v>
       </c>
-      <c r="C4" s="0">
+      <c r="D4" s="0">
         <v>0.16189774468810303</v>
       </c>
-      <c r="D4" s="0">
+      <c r="E4" s="0">
         <v>-0.73568307078561235</v>
       </c>
-      <c r="E4" s="0">
+      <c r="F4" s="0">
         <v>0.015298653023116327</v>
       </c>
-      <c r="F4" s="0">
+      <c r="G4" s="0">
         <v>0.48388327822061694</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0">
         <v>-0.37071725885563156</v>
       </c>
-      <c r="B5" s="0">
+      <c r="C5" s="0">
         <v>0.0013476534267265743</v>
       </c>
-      <c r="C5" s="0">
+      <c r="D5" s="0">
         <v>0.12510887581362518</v>
       </c>
-      <c r="D5" s="0">
+      <c r="E5" s="0">
         <v>-0.53504486018360797</v>
       </c>
-      <c r="E5" s="0">
+      <c r="F5" s="0">
         <v>0.11101834240697142</v>
       </c>
-      <c r="F5" s="0">
+      <c r="G5" s="0">
         <v>0.1970571277100085</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0">
         <v>-0.32193679282951232</v>
       </c>
-      <c r="B6" s="0">
+      <c r="C6" s="0">
         <v>0.0058201308433848045</v>
       </c>
-      <c r="C6" s="0">
+      <c r="D6" s="0">
         <v>0.09083820284274291</v>
       </c>
-      <c r="D6" s="0">
+      <c r="E6" s="0">
         <v>-0.62033137647321956</v>
       </c>
-      <c r="E6" s="0">
+      <c r="F6" s="0">
         <v>0.055686172166231507</v>
       </c>
-      <c r="F6" s="0">
+      <c r="G6" s="0">
         <v>0.30791239371680423</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0">
         <v>-0.3128696714563855</v>
       </c>
-      <c r="B7" s="0">
+      <c r="C7" s="0">
         <v>0.0074537344419594951</v>
       </c>
-      <c r="C7" s="0">
+      <c r="D7" s="0">
         <v>0.085000108907472893</v>
       </c>
-      <c r="D7" s="0">
+      <c r="E7" s="0">
         <v>-0.65627681409009175</v>
       </c>
-      <c r="E7" s="0">
+      <c r="F7" s="0">
         <v>0.039309705979773402</v>
       </c>
-      <c r="F7" s="0">
+      <c r="G7" s="0">
         <v>0.35953666380127092</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="0">
         <v>-0.27077962026187513</v>
       </c>
-      <c r="B8" s="0">
+      <c r="C8" s="0">
         <v>0.021414829680287351</v>
       </c>
-      <c r="C8" s="0">
+      <c r="D8" s="0">
         <v>0.060083339931296109</v>
       </c>
-      <c r="D8" s="0">
+      <c r="E8" s="0">
         <v>-0.58047323657635741</v>
       </c>
-      <c r="E8" s="0">
+      <c r="F8" s="0">
         <v>0.078508485981203344</v>
       </c>
-      <c r="F8" s="0">
+      <c r="G8" s="0">
         <v>0.25406782567911079</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0">
         <v>0.24073346406388768</v>
       </c>
-      <c r="B9" s="0">
+      <c r="C9" s="0">
         <v>0.041649669315030981</v>
       </c>
-      <c r="C9" s="0">
+      <c r="D9" s="0">
         <v>0.044494780730487515</v>
       </c>
-      <c r="D9" s="0">
+      <c r="E9" s="0">
         <v>0.68452418763717526</v>
       </c>
-      <c r="E9" s="0">
+      <c r="F9" s="0">
         <v>0.028989132660429372</v>
       </c>
-      <c r="F9" s="0">
+      <c r="G9" s="0">
         <v>0.40214503389287648</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0">
+        <v>-0.20668838374545503</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.081512206525591629</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.029044660660669908</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-0.51027222742790546</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.13182783038569343</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.16792496434476567</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0">
         <v>-0.18356263486352525</v>
       </c>
-      <c r="B10" s="0">
+      <c r="C11" s="0">
         <v>0.12271728631757317</v>
       </c>
-      <c r="C10" s="0">
+      <c r="D11" s="0">
         <v>0.019890887216869046</v>
       </c>
-      <c r="D10" s="0">
+      <c r="E11" s="0">
         <v>-0.49203524678965072</v>
       </c>
-      <c r="E10" s="0">
+      <c r="F11" s="0">
         <v>0.1485808521298696</v>
       </c>
-      <c r="F10" s="0">
+      <c r="G11" s="0">
         <v>0.14736101959377157</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="0">
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="0">
         <v>-0.13283847054978654</v>
       </c>
-      <c r="B11" s="0">
+      <c r="C12" s="0">
         <v>0.26597351494916044</v>
       </c>
-      <c r="C11" s="0">
+      <c r="D12" s="0">
         <v>0.0036124315331209633</v>
       </c>
-      <c r="D11" s="0">
+      <c r="E12" s="0">
         <v>-0.49079789496616094</v>
       </c>
-      <c r="E11" s="0">
+      <c r="F12" s="0">
         <v>0.14976205592565012</v>
       </c>
-      <c r="F11" s="0">
+      <c r="G12" s="0">
         <v>0.1459928954161166</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="0">
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="0">
         <v>0.13156666261655564</v>
       </c>
-      <c r="B12" s="0">
+      <c r="C13" s="0">
         <v>0.27061871948817673</v>
       </c>
-      <c r="C12" s="0">
+      <c r="D13" s="0">
         <v>0.0032713550936593894</v>
       </c>
-      <c r="D12" s="0">
+      <c r="E13" s="0">
         <v>0.56355347144619428</v>
       </c>
-      <c r="E12" s="0">
+      <c r="F13" s="0">
         <v>0.089781639106618141</v>
       </c>
-      <c r="F12" s="0">
+      <c r="G13" s="0">
         <v>0.23229157957643864</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="0">
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="0">
         <v>0.013848938942451813</v>
       </c>
-      <c r="B13" s="0">
+      <c r="C14" s="0">
         <v>0.90807971910351604</v>
       </c>
-      <c r="C13" s="0">
+      <c r="D14" s="0">
         <v>-0.014091181274313636</v>
       </c>
-      <c r="D13" s="0">
+      <c r="E14" s="0">
         <v>-0.35011345620410883</v>
       </c>
-      <c r="E13" s="0">
+      <c r="F14" s="0">
         <v>0.3213039554134447</v>
       </c>
-      <c r="F13" s="0">
+      <c r="G14" s="0">
         <v>0.012901861242084922</v>
       </c>
     </row>

</xml_diff>